<commit_message>
CBR-425: Update test error messages and Excel test data
Changed error messages in ValidacionAPIItemList.spec.ts to Spanish for itemList size validation. Updated LastmileDeclareRequest.xlsx, ManifestDeclareRequest.xlsx, and ParcelDeclareRequest_v2.xlsx test data files.
</commit_message>
<xml_diff>
--- a/src/testData/archivosExcel/LastmileDeclareRequest.xlsx
+++ b/src/testData/archivosExcel/LastmileDeclareRequest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>idTestCase</t>
   </si>
@@ -67,12 +67,10 @@
     <t>LM2</t>
   </si>
   <si>
-    <t>[{"field": "address","message": "address es obligatorio"},
-{"field": "idUbigeo","message": "idUbigeo es obligatorio"},
-{"field": "email","message": "email es obligatorio"},
-{"field": "mobilePhone","message": "mobilePhone es obligatorio"},
-{"field": "fullName","message": "fullName es obligatorio"},
-{"field": "zipCode","message": "zipCode es obligatorio"}]</t>
+    <t>Alem Corcuera Enco</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
   <si>
     <t>LM3</t>
@@ -87,10 +85,7 @@
     <t>LM4</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>[{"field": "mobilePhone","message": "mobilePhone es obligatorio"}]</t>
+    <t>[{"field":"mobilePhone","message":"mobilePhone: no puede estar en blanco"}]</t>
   </si>
   <si>
     <t>LM5</t>
@@ -111,28 +106,28 @@
     <t>LM7</t>
   </si>
   <si>
-    <t>Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - LimaLima Av. Los Olivos 123</t>
+    <t>Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Ol</t>
   </si>
   <si>
     <t>LM8</t>
   </si>
   <si>
-    <t>Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - LimaLima Av. Los Olivos 1241</t>
-  </si>
-  <si>
-    <t>[{"field": "address","message": "address: máximo 250 caracteres"}]</t>
+    <t>Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Olivos 1234, Dpto. 201 - Lima Av. Los Oli</t>
+  </si>
+  <si>
+    <t>[{"field":"address","message":"address: máximo 200 caracteres"}]</t>
   </si>
   <si>
     <t>LM9</t>
   </si>
   <si>
-    <t>[{"field": "address","message": "address es obligatorio"}]</t>
+    <t>[{"field":"address","message":"address: No debe estar vacío"}]</t>
   </si>
   <si>
     <t>LM10</t>
   </si>
   <si>
-    <t>Gabriel Alessandro Benites BesadaGabriel Alessandro Benites BesadaGabriel Alesss Besada123451234512345123451111111111111</t>
+    <t>Gabriel Alessandro Benites BesadaGabriel Alessandro Benites BesadaGabriel Alesss Besada1234512345123</t>
   </si>
   <si>
     <t>Av. Los Olivos 1234, Dpto. 201</t>
@@ -141,100 +136,46 @@
     <t>LM11</t>
   </si>
   <si>
-    <t>Gabriel Alessandro Benites BesadaGabriel Alessandro Benites BesadaGabriel Alesss Besada1234512345123451234511111111111112</t>
+    <t>Gabriel Alessandro Benites BesadaGabriel Alessandro Benites BesadaGabriel Alesss Besada12345123451234</t>
   </si>
   <si>
     <t>Av. Los Olivos 1234, Dpto. 202</t>
   </si>
   <si>
+    <t>[{"field":"fullName","message":"fullName: máximo 100 caracteres"}]</t>
+  </si>
+  <si>
     <t>LM12</t>
   </si>
   <si>
     <t>Av. Los Olivos 1234, Dpto. 203</t>
   </si>
   <si>
-    <t>[{"field": "fullName","message": "fullName es obligatorio"}]</t>
+    <t>[{"field":"fullName","message":"fullName: no puede estar en blanco"}]</t>
   </si>
   <si>
     <t>LM13</t>
   </si>
   <si>
+    <t>LIMA32LIMA32LIMA32LIMA32LIMA3212</t>
+  </si>
+  <si>
+    <t>{"status": "ACCEPTED","message": "Updated request accepted"}</t>
+  </si>
+  <si>
     <t>LM14</t>
   </si>
   <si>
-    <t>gabriel.benites.1998.lima.marketing.ventas.2025.oficial.lima.peru.team.contacto.oficina00123456consultoresdigita@example.com</t>
-  </si>
-  <si>
-    <t>LIMA33</t>
-  </si>
-  <si>
-    <t>{"field": "email","message": "email: máximo 120 caracteres"}</t>
+    <t>1LIMA32LIMA32LIMA32LIMA32LIMA3213</t>
+  </si>
+  <si>
+    <t>[{"field": "zipCode","message": "zipCode: máximo 32 caracteres"}]</t>
   </si>
   <si>
     <t>LM15</t>
   </si>
   <si>
-    <t>gabriel.benites.1998.lima.marketing.ventas.2025.oficial.lima.peru.team.contacto.oficina00@consultores-digitales-peru.com</t>
-  </si>
-  <si>
-    <t>LIMA34</t>
-  </si>
-  <si>
-    <t>[{"field":"email","message":"email debe ser válido"}]</t>
-  </si>
-  <si>
-    <t>LM16</t>
-  </si>
-  <si>
-    <t>LIMA35</t>
-  </si>
-  <si>
-    <t>[{"field": "email","message": "email es obligatorio"}]</t>
-  </si>
-  <si>
-    <t>LM17</t>
-  </si>
-  <si>
-    <t>LM18</t>
-  </si>
-  <si>
-    <t>[{"field": "idUbigeo","message": "idUbigeo: máximo 4 caracteres"}]</t>
-  </si>
-  <si>
-    <t>LM19</t>
-  </si>
-  <si>
-    <t>[{"field": "idUbigeo","message": "idUbigeo es obligatorio"}]</t>
-  </si>
-  <si>
-    <t>LM20</t>
-  </si>
-  <si>
-    <t>LIMA32LIMA32LIMA32LIMA32LIMA3212</t>
-  </si>
-  <si>
-    <t>{"status": "ACCEPTED","message": "Updated request accepted"}</t>
-  </si>
-  <si>
-    <t>LM21</t>
-  </si>
-  <si>
-    <t>1LIMA32LIMA32LIMA32LIMA32LIMA3213</t>
-  </si>
-  <si>
-    <t>[{"field": "zipCode","message": "zipCode: máximo 32 caracteres"}]</t>
-  </si>
-  <si>
-    <t>LM22</t>
-  </si>
-  <si>
-    <t>[{"field": "zipCode","message": "zipCode es obligatorio"}]</t>
-  </si>
-  <si>
-    <t>LM23</t>
-  </si>
-  <si>
-    <t>[{"field":"address","message":"address es obligatorio"},{"field":"fullName","message":"fullName es obligatorio"},{"field":"idUbigeo","message":"idUbigeo es obligatorio"},{"field":"email","message":"email es obligatorio"},{"field":"mobilePhone","message":"mobilePhone es obligatorio"},{"field":"zipCode","message":"zipCode es obligatorio"}]</t>
+    <t>[{"field":"address","message":"address: No debe estar vacío"},{"field":"fullName","message":"fullName: no puede estar en blanco"},{"field":"mobilePhone","message":"mobilePhone: no puede estar en blanco"}]</t>
   </si>
 </sst>
 </file>
@@ -258,18 +199,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -292,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -306,10 +241,6 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -588,7 +519,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="3">
-        <f>51987654321</f>
+        <f t="shared" ref="F2:F4" si="1">51987654321</f>
         <v>51987654321</v>
       </c>
       <c r="G2" s="1">
@@ -608,56 +539,71 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="1"/>
+        <v>51987654321</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="I3" s="1">
-        <v>400.0</v>
+        <v>202.0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="6">
-        <f>51987654321</f>
-        <v>51987654321</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1501.0</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>51987654321</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1501.0</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1">
         <v>202.0</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>21</v>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -672,7 +618,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1">
         <v>1501.0</v>
@@ -703,7 +649,7 @@
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="1">
@@ -735,7 +681,7 @@
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="1">
@@ -768,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ref="F8:F13" si="1">51987654321</f>
+        <f t="shared" ref="F8:F15" si="2">51987654321</f>
         <v>51987654321</v>
       </c>
       <c r="G8" s="1">
@@ -801,7 +747,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51987654321</v>
       </c>
       <c r="G9" s="1">
@@ -828,13 +774,13 @@
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51987654321</v>
       </c>
       <c r="G10" s="1">
@@ -867,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51987654321</v>
       </c>
       <c r="G11" s="1">
@@ -884,56 +830,56 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" si="1"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1501.0</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>51987654321</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1501.0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="1">
         <v>400.0</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>21</v>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51987654321</v>
       </c>
       <c r="G13" s="1">
@@ -946,32 +892,45 @@
         <v>400.0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5">
-        <v>400.0</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>21</v>
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>51987654321</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1501.0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -983,307 +942,43 @@
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" ref="F15:F23" si="2">51987654321</f>
+        <f t="shared" si="2"/>
         <v>51987654321</v>
       </c>
       <c r="G15" s="1">
         <v>1501.0</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I15" s="1">
         <v>400.0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1501.0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="1">
         <v>400.0</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1501.0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="1">
-        <v>400.0</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1501.0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="1">
-        <v>202.0</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G19" s="1">
-        <v>15101.0</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="1">
-        <v>400.0</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="1">
-        <v>400.0</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1501.0</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="1">
-        <v>202.0</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1501.0</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="1">
-        <v>400.0</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="2"/>
-        <v>51987654321</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1501.0</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="1">
-        <v>400.0</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="1">
-        <v>400.0</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>